<commit_message>
add updated notes on rmg runs of nheptane
</commit_message>
<xml_diff>
--- a/nheptane/rmg_runs.xlsx
+++ b/nheptane/rmg_runs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\moon\autoscience\autoscience\nheptane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D938FB9-0A67-4E9C-842E-F9AFE01204F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3139BD-4988-4F76-9DCF-3648CFBF6B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{089DF937-5BC5-4D2A-A52F-D896C99C9EE6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{089DF937-5BC5-4D2A-A52F-D896C99C9EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Date run</t>
   </si>
@@ -68,7 +68,25 @@
     <t>/work/westgroup/harris.se/autoscience/nheptane_iter0He2</t>
   </si>
   <si>
-    <t>Copy of #1 but ran 24 hours</t>
+    <t>Copy of #1 but ran 48 hours</t>
+  </si>
+  <si>
+    <t>copy of #1 but with additional library with 10 new thermos</t>
+  </si>
+  <si>
+    <t>/work/westgroup/harris.se/autoscience/nhept_iter1</t>
+  </si>
+  <si>
+    <t>/work/westgroup/harris.se/autoscience/nheptane4</t>
+  </si>
+  <si>
+    <t>copy of #1 but using latest RMG-Py/RMG-database, and 7 day time limit</t>
+  </si>
+  <si>
+    <t>copy of #1 but using latest RMG-Py/RMG-database, and 24 hour time limit</t>
+  </si>
+  <si>
+    <t>/work/westgroup/harris.se/autoscience/nheptane5</t>
   </si>
 </sst>
 </file>
@@ -421,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885FE852-4645-438A-92D8-C3DC52368D68}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,6 +520,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44610</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44683</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44683</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>